<commit_message>
code should be final
</commit_message>
<xml_diff>
--- a/Lab3/data.xlsx
+++ b/Lab3/data.xlsx
@@ -8,20 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanKennedy/Desktop/School/Third Year/Fall Semester/CS-3353/CS-3353-Algorithms/Lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85A006FE-ED70-C649-8A25-3DED93E33CE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C950185-4FC0-5440-A0D8-BA31A6490271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="20300" xr2:uid="{8DB08708-3E1B-AC47-97D6-048F023EFFA7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20300" xr2:uid="{8DB08708-3E1B-AC47-97D6-048F023EFFA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$11:$B$19</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$11:$C$19</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$B$11:$B$19</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$C$11:$C$19</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$41</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$42:$A$50</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$41</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$42:$B$50</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$41</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$42:$C$50</definedName>
+    <definedName name="_xlchart.v2.10" hidden="1">Sheet1!$C$41</definedName>
+    <definedName name="_xlchart.v2.11" hidden="1">Sheet1!$C$42:$C$50</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">Sheet1!$A$41</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">Sheet1!$A$42:$A$50</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">Sheet1!$B$41</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">Sheet1!$B$42:$B$50</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
     <t>Dynamic Programming</t>
   </si>
@@ -60,13 +68,16 @@
     <t>Naïve</t>
   </si>
   <si>
-    <t>time taken (s)</t>
+    <t>time taken (ms)</t>
   </si>
   <si>
-    <t>Naïve time - DP time</t>
+    <t>Nodes</t>
   </si>
   <si>
-    <t>Naïve - DP</t>
+    <t>n^2 * 2^n</t>
+  </si>
+  <si>
+    <t>!n</t>
   </si>
 </sst>
 </file>
@@ -111,12 +122,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -149,6 +162,46 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Dyanmic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Programming and </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Naïve</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> time vs. Number of Nodes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -181,14 +234,25 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dynamic Programming</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -197,67 +261,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$B$19</c:f>
+              <c:f>Sheet1!$A$22:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -290,51 +298,157 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$11:$C$19</c:f>
+              <c:f>Sheet1!$B$22:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.5638999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4469000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>4.8508999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>9.2711000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>0.19899800000000001</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.38763500000000001</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.84530899999999998</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>1.6068499999999999</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>4.0311300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B874-8E4A-985A-ECC17F5F5907}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Naïve</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$22:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>116</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>380</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1122</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3094</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8136</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20664</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51110</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>123794</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$22:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>1.9904000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3638999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42018499999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1115200000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.816700000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>148.876</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1397.63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12895.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>147421</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-098E-7E49-BA06-06C48DF97248}"/>
+              <c16:uniqueId val="{00000001-B874-8E4A-985A-ECC17F5F5907}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -342,30 +456,76 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="840292608"/>
-        <c:axId val="840294240"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="840292608"/>
+        <c:smooth val="0"/>
+        <c:axId val="586104111"/>
+        <c:axId val="626148655"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="586104111"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -375,8 +535,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -403,12 +563,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="840294240"/>
+        <c:crossAx val="626148655"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="840294240"/>
+        <c:axId val="626148655"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,6 +591,520 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in Milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="586104111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Dynamic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Programming number of operations and n^2*2^n vs. number of nodes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dynamic Programming</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$32:$A$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$32:$B$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1122</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3094</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8136</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20664</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51110</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>123794</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7CE8-8349-9F10-999F396A95E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>n^2 * 2^n</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$32:$A$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$32:$C$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6272</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41472</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>102400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>247808</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>589823</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7CE8-8349-9F10-999F396A95E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="642355583"/>
+        <c:axId val="640043471"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="642355583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -437,8 +1114,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -465,9 +1142,68 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="840292608"/>
+        <c:crossAx val="640043471"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="640043471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="642355583"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -477,6 +1213,521 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Naive</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> number of operations and n! vs. number of nodes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Naïve</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$42:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$42:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5040</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40320</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>362880</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3628800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39916800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>479001600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C7A5-8F47-A61B-8A0F5F7EC8CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>!n</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$42:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$42:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5040</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40320</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>362880</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3628800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39916800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>479001600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C7A5-8F47-A61B-8A0F5F7EC8CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="645862863"/>
+        <c:axId val="644909247"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="645862863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="644909247"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="644909247"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="645862863"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -554,8 +1805,88 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -582,8 +1913,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -663,6 +1994,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -673,6 +2009,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -684,7 +2025,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -704,6 +2045,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -716,10 +2060,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -759,23 +2103,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -880,8 +2223,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1013,24 +2356,417 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1040,17 +2776,644 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="25000"/>
             <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1074,23 +3437,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{918ACAB3-5278-0148-8E82-37F373075B1D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{672F9E23-A0E8-E848-81BB-0DCC0453DD35}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1103,6 +3466,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A061846-E2CC-7242-A8BF-13002BCF5496}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F72C6549-6897-D145-B461-3362909156C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1408,566 +3843,751 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B20E59-11B9-1D48-9BED-FF3C52114FDF}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="1" max="1" width="19.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>24</v>
       </c>
-      <c r="D2" s="4">
-        <v>4.2469000000000003E-5</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="2">
+        <v>1.9904000000000002E-2</v>
+      </c>
+      <c r="E2" s="1">
         <f>FACT(B2)</f>
         <v>24</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>644.56399999999996</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>120</v>
       </c>
-      <c r="D3">
-        <v>1.4229800000000001E-4</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:F10" si="0">FACT(B3)</f>
+      <c r="D3" s="1">
+        <v>7.3638999999999996E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E10" si="0">FACT(B3)</f>
         <v>120</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>648.73800000000006</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>720</v>
       </c>
-      <c r="D4">
-        <v>7.1756200000000004E-4</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="1">
+        <v>0.42018499999999998</v>
+      </c>
+      <c r="E4" s="1">
         <f t="shared" si="0"/>
         <v>720</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>702.64200000000005</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>7</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>5040</v>
       </c>
-      <c r="D5">
-        <v>4.7633099999999998E-3</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="1">
+        <v>2.1115200000000001</v>
+      </c>
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>5040</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>714.23900000000003</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>40320</v>
       </c>
-      <c r="D6">
-        <v>2.34562E-2</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="1">
+        <v>14.816700000000001</v>
+      </c>
+      <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>40320</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>715.34199999999998</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>9</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>362880</v>
       </c>
-      <c r="D7">
-        <v>0.12626699999999999</v>
-      </c>
-      <c r="E7">
+      <c r="D7" s="1">
+        <v>148.876</v>
+      </c>
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>362880</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>720.12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>10</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>3628800</v>
       </c>
-      <c r="D8">
-        <v>1.17702</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="1">
+        <v>1397.63</v>
+      </c>
+      <c r="E8" s="3">
         <f t="shared" si="0"/>
         <v>3628800</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>726.37400000000002</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>11</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>39916800</v>
       </c>
-      <c r="D9">
-        <v>11.954599999999999</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="D9" s="1">
+        <v>12895.7</v>
+      </c>
+      <c r="E9" s="3">
         <f t="shared" si="0"/>
         <v>39916800</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>735.36199999999997</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>12</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>479001600</v>
       </c>
-      <c r="D10" s="3">
-        <v>158.376</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="D10" s="4">
+        <v>147421</v>
+      </c>
+      <c r="E10" s="4">
         <f t="shared" si="0"/>
         <v>479001600</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="4">
         <v>739.68</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>4</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>30</v>
       </c>
-      <c r="D11" s="4">
-        <v>5.9327999999999998E-5</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="D11" s="2">
+        <v>2.5638999999999999E-2</v>
+      </c>
+      <c r="E11" s="5">
         <f>POWER(2,B11)*POWER(B11,2)</f>
         <v>256</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>644.56399999999996</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>5</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>116</v>
       </c>
-      <c r="D12" s="4">
-        <v>6.5964999999999996E-5</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" ref="E12:F19" si="1">POWER(2,B12)*POWER(B12,2)</f>
+      <c r="D12" s="2">
+        <v>2.4469000000000001E-2</v>
+      </c>
+      <c r="E12" s="5">
+        <f>POWER(2,B12)*POWER(B12,2)</f>
         <v>800</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>648.73800000000006</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>6</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>380</v>
       </c>
-      <c r="D13">
-        <v>1.13835E-4</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="1"/>
+      <c r="D13" s="1">
+        <v>4.8508999999999997E-2</v>
+      </c>
+      <c r="E13" s="5">
+        <f>POWER(2,B13)*POWER(B13,2)</f>
         <v>2304</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>702.64200000000005</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>7</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>1122</v>
       </c>
-      <c r="D14">
-        <v>1.6732699999999999E-4</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="1"/>
+      <c r="D14" s="1">
+        <v>9.2711000000000002E-2</v>
+      </c>
+      <c r="E14" s="5">
+        <f>POWER(2,B14)*POWER(B14,2)</f>
         <v>6272</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>714.23900000000003</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>8</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>3094</v>
       </c>
-      <c r="D15">
-        <v>3.4862400000000002E-4</v>
-      </c>
-      <c r="E15" s="1">
-        <f t="shared" si="1"/>
+      <c r="D15" s="1">
+        <v>0.19899800000000001</v>
+      </c>
+      <c r="E15" s="5">
+        <f>POWER(2,B15)*POWER(B15,2)</f>
         <v>16384</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>715.34199999999998</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>9</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>8136</v>
       </c>
-      <c r="D16">
-        <v>5.0790099999999995E-4</v>
-      </c>
-      <c r="E16" s="1">
-        <f t="shared" si="1"/>
+      <c r="D16" s="1">
+        <v>0.38763500000000001</v>
+      </c>
+      <c r="E16" s="5">
+        <f>POWER(2,B16)*POWER(B16,2)</f>
         <v>41472</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>720.12</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>10</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>20664</v>
       </c>
-      <c r="D17">
-        <v>7.4936700000000002E-4</v>
-      </c>
-      <c r="E17" s="1">
-        <f t="shared" si="1"/>
+      <c r="D17" s="1">
+        <v>0.84530899999999998</v>
+      </c>
+      <c r="E17" s="5">
+        <f>POWER(2,B17)*POWER(B17,2)</f>
         <v>102400</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>726.37400000000002</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>11</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>51110</v>
       </c>
-      <c r="D18">
-        <v>1.64065E-3</v>
-      </c>
-      <c r="E18" s="1">
-        <f t="shared" si="1"/>
+      <c r="D18" s="1">
+        <v>1.6068499999999999</v>
+      </c>
+      <c r="E18" s="5">
+        <f>POWER(2,B18)*POWER(B18,2)</f>
         <v>247808</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>735.36199999999997</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>12</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>123794</v>
       </c>
-      <c r="D19">
-        <v>3.7363299999999999E-3</v>
-      </c>
-      <c r="E19" s="1">
-        <f t="shared" si="1"/>
+      <c r="D19" s="1">
+        <v>4.0311300000000001</v>
+      </c>
+      <c r="E19" s="5">
+        <f>POWER(2,B19)*POWER(B19,2)</f>
         <v>589824</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>739.68</v>
       </c>
     </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="1">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2.5638999999999999E-2</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.9904000000000002E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>5</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2.4469000000000001E-2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>7.3638999999999996E-2</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>6</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4.8508999999999997E-2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.42018499999999998</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1">
+        <v>9.2711000000000002E-2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2.1115200000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.19899800000000001</v>
+      </c>
+      <c r="C26" s="1">
+        <v>14.816700000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>9</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B27" s="1">
+        <v>0.38763500000000001</v>
+      </c>
+      <c r="C27" s="1">
+        <v>148.876</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>10</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.84530899999999998</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1397.63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>11</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.6068499999999999</v>
+      </c>
+      <c r="C29" s="1">
+        <v>12895.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>12</v>
+      </c>
+      <c r="B30" s="1">
+        <v>4.0311300000000001</v>
+      </c>
+      <c r="C30" s="3">
+        <v>147421</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <f>C2-C11</f>
-        <v>-6</v>
-      </c>
-      <c r="B23" s="4">
-        <f>D2-D11</f>
-        <v>-1.6858999999999996E-5</v>
-      </c>
-      <c r="C23">
+      <c r="B31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
         <v>4</v>
       </c>
-      <c r="D23" s="4">
-        <v>5.9327999999999998E-5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <f>C3-C12</f>
+      <c r="B32" s="1">
+        <v>30</v>
+      </c>
+      <c r="C32" s="6">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1">
+        <v>116</v>
+      </c>
+      <c r="C33" s="6">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>6</v>
+      </c>
+      <c r="B34" s="1">
+        <v>380</v>
+      </c>
+      <c r="C34" s="6">
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>7</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1122</v>
+      </c>
+      <c r="C35" s="6">
+        <v>6272</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>8</v>
+      </c>
+      <c r="B36" s="1">
+        <v>3094</v>
+      </c>
+      <c r="C36" s="6">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1">
+        <v>8136</v>
+      </c>
+      <c r="C37" s="6">
+        <v>41472</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>10</v>
+      </c>
+      <c r="B38" s="1">
+        <v>20664</v>
+      </c>
+      <c r="C38" s="6">
+        <v>102400</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>11</v>
+      </c>
+      <c r="B39" s="1">
+        <v>51110</v>
+      </c>
+      <c r="C39" s="6">
+        <v>247808</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1">
+        <v>123794</v>
+      </c>
+      <c r="C40" s="6">
+        <v>589823</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
         <v>4</v>
       </c>
-      <c r="B24" s="4">
-        <f>D3-D12</f>
-        <v>7.6333000000000016E-5</v>
-      </c>
-      <c r="C24">
+      <c r="B42" s="3">
+        <v>24</v>
+      </c>
+      <c r="C42" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
         <v>5</v>
       </c>
-      <c r="D24" s="4">
-        <v>6.5964999999999996E-5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <f t="shared" ref="A25:A31" si="2">C4-C13</f>
-        <v>340</v>
-      </c>
-      <c r="B25">
-        <f>D4-D13</f>
-        <v>6.0372700000000008E-4</v>
-      </c>
-      <c r="C25">
+      <c r="B43" s="3">
+        <v>120</v>
+      </c>
+      <c r="C43" s="3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
         <v>6</v>
       </c>
-      <c r="D25">
-        <v>1.13835E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <f t="shared" si="2"/>
-        <v>3918</v>
-      </c>
-      <c r="B26" s="4">
-        <f t="shared" ref="B26:B31" si="3">D5-D14</f>
-        <v>4.5959829999999997E-3</v>
-      </c>
-      <c r="C26">
+      <c r="B44" s="3">
+        <v>720</v>
+      </c>
+      <c r="C44" s="3">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
         <v>7</v>
       </c>
-      <c r="D26">
-        <v>1.6732699999999999E-4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <f t="shared" si="2"/>
-        <v>37226</v>
-      </c>
-      <c r="B27">
-        <f t="shared" si="3"/>
-        <v>2.3107576000000001E-2</v>
-      </c>
-      <c r="C27">
+      <c r="B45" s="3">
+        <v>5040</v>
+      </c>
+      <c r="C45" s="3">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
         <v>8</v>
       </c>
-      <c r="D27">
-        <v>3.4862400000000002E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <f t="shared" si="2"/>
-        <v>354744</v>
-      </c>
-      <c r="B28" s="4">
-        <f t="shared" si="3"/>
-        <v>0.12575909899999999</v>
-      </c>
-      <c r="C28">
+      <c r="B46" s="3">
+        <v>40320</v>
+      </c>
+      <c r="C46" s="3">
+        <v>40320</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
         <v>9</v>
       </c>
-      <c r="D28">
-        <v>5.0790099999999995E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <f t="shared" si="2"/>
-        <v>3608136</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="3"/>
-        <v>1.1762706329999999</v>
-      </c>
-      <c r="C29">
+      <c r="B47" s="3">
+        <v>362880</v>
+      </c>
+      <c r="C47" s="3">
+        <v>362880</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
         <v>10</v>
       </c>
-      <c r="D29">
-        <v>7.4936700000000002E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <f t="shared" si="2"/>
-        <v>39865690</v>
-      </c>
-      <c r="B30" s="4">
-        <f t="shared" si="3"/>
-        <v>11.952959349999999</v>
-      </c>
-      <c r="C30">
+      <c r="B48" s="3">
+        <v>3628800</v>
+      </c>
+      <c r="C48" s="3">
+        <v>3628800</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
         <v>11</v>
       </c>
-      <c r="D30">
-        <v>1.64065E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <f t="shared" si="2"/>
-        <v>478877806</v>
-      </c>
-      <c r="B31">
-        <f t="shared" si="3"/>
-        <v>158.37226367</v>
-      </c>
-      <c r="C31">
+      <c r="B49" s="3">
+        <v>39916800</v>
+      </c>
+      <c r="C49" s="3">
+        <v>39916800</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>12</v>
       </c>
-      <c r="D31">
-        <v>3.7363299999999999E-3</v>
+      <c r="B50" s="3">
+        <v>479001600</v>
+      </c>
+      <c r="C50" s="3">
+        <v>479001600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>